<commit_message>
November changes including resque background job and refactored code due to ReCharge API changes
</commit_message>
<xml_diff>
--- a/update_prepaid_config.xlsx
+++ b/update_prepaid_config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FWallace/Shopify/three_months/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1782430D-2095-054F-8B96-27250184D424}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3C54843-47EB-7A45-A35F-A67812AB277C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{48A45615-4120-754D-B82C-99CF12962432}"/>
+    <workbookView xWindow="3820" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{48A45615-4120-754D-B82C-99CF12962432}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>title</t>
   </si>
@@ -39,7 +39,10 @@
     <t>product_collection</t>
   </si>
   <si>
-    <t>Desert Sage - 5 Item</t>
+    <t>3 MONTHS</t>
+  </si>
+  <si>
+    <t>Print Paradise - 5 Items</t>
   </si>
 </sst>
 </file>
@@ -47,7 +50,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="######00000"/>
+    <numFmt numFmtId="164" formatCode="######00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -80,7 +83,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,7 +401,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,13 +431,13 @@
         <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>197983830034</v>
+        <v>23729012754</v>
       </c>
       <c r="C2" s="1">
-        <v>1788451618834</v>
+        <v>177939546130</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>